<commit_message>
updating and removing papers + data extraction that do not meet criteria
</commit_message>
<xml_diff>
--- a/data extraction /lit search metadata /wos176_final.xlsx
+++ b/data extraction /lit search metadata /wos176_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /lit search metadata /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB8E27F-8B80-C140-8234-3B55A3BE853E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26669599-C536-8C46-8936-E12AEF3E768A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28820" yWindow="-10880" windowWidth="23980" windowHeight="10600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-19940" windowWidth="23980" windowHeight="10600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wos176_final" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1673" uniqueCount="937">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1676" uniqueCount="938">
   <si>
     <t>label</t>
   </si>
@@ -2630,15 +2630,9 @@
     <t>figure 1,2</t>
   </si>
   <si>
-    <t>unsure about the temperature variation pattern in this study</t>
-  </si>
-  <si>
     <t>figure 3, 4</t>
   </si>
   <si>
-    <t>missing n for figure 3</t>
-  </si>
-  <si>
     <t>figure 2, 3</t>
   </si>
   <si>
@@ -2832,6 +2826,15 @@
   </si>
   <si>
     <t xml:space="preserve">results report simply model based data </t>
+  </si>
+  <si>
+    <t>reared at fluctuating temperatures, and exposed to constant temperatures for thermal performance curve (acclimation?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no sample size or error measurement reported, response listed as percentage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pulse/press experiment, can't seem to find sample size but there are error bars indicated standard deviation </t>
   </si>
 </sst>
 </file>
@@ -3693,8 +3696,8 @@
   <dimension ref="A1:R119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26:XFD26"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3752,7 +3755,7 @@
         <v>10</v>
       </c>
       <c r="R1" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -4657,7 +4660,7 @@
         <v>23</v>
       </c>
       <c r="N23" t="s">
-        <v>856</v>
+        <v>859</v>
       </c>
       <c r="O23" t="s">
         <v>864</v>
@@ -4665,8 +4668,11 @@
       <c r="P23" t="s">
         <v>866</v>
       </c>
+      <c r="Q23" t="s">
+        <v>935</v>
+      </c>
       <c r="R23" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
     </row>
     <row r="24" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4719,7 +4725,7 @@
         <v>866</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
     </row>
     <row r="25" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4772,7 +4778,7 @@
         <v>866</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
     </row>
     <row r="26" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4825,7 +4831,7 @@
         <v>866</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
@@ -4869,7 +4875,7 @@
         <v>23</v>
       </c>
       <c r="N27" t="s">
-        <v>856</v>
+        <v>859</v>
       </c>
       <c r="O27" t="s">
         <v>867</v>
@@ -4878,7 +4884,7 @@
         <v>866</v>
       </c>
       <c r="Q27" t="s">
-        <v>869</v>
+        <v>937</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
@@ -4925,13 +4931,13 @@
         <v>856</v>
       </c>
       <c r="O28" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="P28" t="s">
         <v>866</v>
       </c>
-      <c r="Q28" t="s">
-        <v>871</v>
+      <c r="R28" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
@@ -5033,6 +5039,9 @@
       <c r="P30" t="s">
         <v>866</v>
       </c>
+      <c r="R30" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -5078,13 +5087,13 @@
         <v>856</v>
       </c>
       <c r="O31" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="P31" t="s">
         <v>866</v>
       </c>
       <c r="Q31" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
@@ -5131,13 +5140,13 @@
         <v>856</v>
       </c>
       <c r="O32" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="P32" t="s">
         <v>866</v>
       </c>
       <c r="Q32" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
@@ -5184,13 +5193,13 @@
         <v>856</v>
       </c>
       <c r="O33" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="P33" t="s">
         <v>866</v>
       </c>
       <c r="Q33" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
@@ -5243,7 +5252,7 @@
         <v>866</v>
       </c>
       <c r="Q34" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
     </row>
     <row r="35" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5293,7 +5302,7 @@
         <v>866</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
@@ -5346,7 +5355,7 @@
         <v>866</v>
       </c>
       <c r="Q36" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
     </row>
     <row r="37" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5393,13 +5402,13 @@
         <v>856</v>
       </c>
       <c r="O37" s="2" t="s">
+        <v>880</v>
+      </c>
+      <c r="P37" s="2" t="s">
         <v>882</v>
       </c>
-      <c r="P37" s="2" t="s">
-        <v>884</v>
-      </c>
       <c r="Q37" s="2" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
@@ -5446,13 +5455,13 @@
         <v>856</v>
       </c>
       <c r="O38" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="P38" t="s">
         <v>866</v>
       </c>
       <c r="Q38" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
@@ -5552,7 +5561,7 @@
         <v>866</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
@@ -5605,7 +5614,7 @@
         <v>866</v>
       </c>
       <c r="Q41" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.2">
@@ -5649,16 +5658,19 @@
         <v>23</v>
       </c>
       <c r="N42" t="s">
-        <v>856</v>
+        <v>859</v>
       </c>
       <c r="O42" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="P42" t="s">
         <v>866</v>
       </c>
+      <c r="Q42" t="s">
+        <v>936</v>
+      </c>
       <c r="R42" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
     </row>
     <row r="43" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5708,7 +5720,7 @@
         <v>866</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
@@ -5755,7 +5767,7 @@
         <v>856</v>
       </c>
       <c r="O44" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="P44" t="s">
         <v>866</v>
@@ -5855,13 +5867,13 @@
         <v>856</v>
       </c>
       <c r="O46" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="P46" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="Q46" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">
@@ -5908,13 +5920,13 @@
         <v>856</v>
       </c>
       <c r="O47" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="P47" t="s">
         <v>866</v>
       </c>
       <c r="Q47" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
     </row>
     <row r="48" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5964,7 +5976,7 @@
         <v>866</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
@@ -6011,7 +6023,7 @@
         <v>856</v>
       </c>
       <c r="O49" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="P49" t="s">
         <v>866</v>
@@ -6061,7 +6073,7 @@
         <v>856</v>
       </c>
       <c r="O50" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="P50" t="s">
         <v>866</v>
@@ -6111,13 +6123,13 @@
         <v>856</v>
       </c>
       <c r="O51" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="P51" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="Q51" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
     </row>
     <row r="52" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6164,7 +6176,7 @@
         <v>859</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
@@ -6211,7 +6223,7 @@
         <v>856</v>
       </c>
       <c r="O53" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="P53" t="s">
         <v>866</v>
@@ -6261,7 +6273,7 @@
         <v>859</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="55" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6308,7 +6320,7 @@
         <v>859</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
@@ -6355,13 +6367,13 @@
         <v>856</v>
       </c>
       <c r="O56" s="3" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="P56" t="s">
         <v>866</v>
       </c>
       <c r="Q56" s="3" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
     </row>
     <row r="57" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6408,7 +6420,7 @@
         <v>859</v>
       </c>
       <c r="Q57" s="1" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
@@ -6455,7 +6467,7 @@
         <v>856</v>
       </c>
       <c r="O58" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="P58" t="s">
         <v>866</v>
@@ -6506,13 +6518,13 @@
         <v>856</v>
       </c>
       <c r="O59" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="P59" t="s">
         <v>866</v>
       </c>
       <c r="Q59" s="3" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
     </row>
     <row r="60" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6559,7 +6571,7 @@
         <v>859</v>
       </c>
       <c r="Q60" s="1" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
@@ -6606,13 +6618,13 @@
         <v>856</v>
       </c>
       <c r="O61" s="3" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="P61" s="3" t="s">
         <v>866</v>
       </c>
       <c r="Q61" s="3" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
     </row>
     <row r="62" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6659,7 +6671,7 @@
         <v>859</v>
       </c>
       <c r="Q62" s="1" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
@@ -6706,7 +6718,7 @@
         <v>856</v>
       </c>
       <c r="O63" s="3" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="P63" s="3" t="s">
         <v>866</v>
@@ -6756,13 +6768,13 @@
         <v>856</v>
       </c>
       <c r="O64" s="3" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="P64" s="3" t="s">
         <v>866</v>
       </c>
       <c r="Q64" s="3" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
@@ -6809,7 +6821,7 @@
         <v>856</v>
       </c>
       <c r="O65" s="3" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="P65" s="3" t="s">
         <v>866</v>
@@ -6859,7 +6871,7 @@
         <v>856</v>
       </c>
       <c r="O66" s="3" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="P66" s="3" t="s">
         <v>866</v>
@@ -6915,7 +6927,7 @@
         <v>866</v>
       </c>
       <c r="Q67" s="3" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
     </row>
     <row r="68" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6965,7 +6977,7 @@
         <v>866</v>
       </c>
       <c r="Q68" s="1" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
     </row>
     <row r="69" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7015,7 +7027,7 @@
         <v>866</v>
       </c>
       <c r="Q69" s="1" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
     </row>
     <row r="70" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7065,7 +7077,7 @@
         <v>866</v>
       </c>
       <c r="Q70" s="1" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
     </row>
     <row r="71" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7162,7 +7174,7 @@
         <v>866</v>
       </c>
       <c r="Q72" s="1" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="73" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7212,7 +7224,7 @@
         <v>866</v>
       </c>
       <c r="Q73" s="1" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
     </row>
     <row r="74" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7259,10 +7271,10 @@
         <v>859</v>
       </c>
       <c r="P74" s="1" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="Q74" s="1" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
     </row>
     <row r="75" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -7514,10 +7526,10 @@
         <v>859</v>
       </c>
       <c r="P80" s="1" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="Q80" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
     </row>
     <row r="81" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8311,10 +8323,10 @@
         <v>859</v>
       </c>
       <c r="P99" s="1" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="Q99" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
     </row>
     <row r="100" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8408,10 +8420,10 @@
         <v>859</v>
       </c>
       <c r="P101" s="1" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="Q101" s="1" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="102" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8458,10 +8470,10 @@
         <v>859</v>
       </c>
       <c r="P102" s="1" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="Q102" s="1" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="103" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8508,10 +8520,10 @@
         <v>859</v>
       </c>
       <c r="P103" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="Q103" s="1" t="s">
         <v>917</v>
-      </c>
-      <c r="Q103" s="1" t="s">
-        <v>919</v>
       </c>
     </row>
     <row r="104" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8558,10 +8570,10 @@
         <v>859</v>
       </c>
       <c r="P104" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="Q104" s="1" t="s">
         <v>917</v>
-      </c>
-      <c r="Q104" s="1" t="s">
-        <v>919</v>
       </c>
     </row>
     <row r="105" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8608,10 +8620,10 @@
         <v>859</v>
       </c>
       <c r="P105" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="Q105" s="1" t="s">
         <v>917</v>
-      </c>
-      <c r="Q105" s="1" t="s">
-        <v>919</v>
       </c>
     </row>
     <row r="106" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8658,10 +8670,10 @@
         <v>859</v>
       </c>
       <c r="P106" s="1" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="Q106" s="1" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
     </row>
     <row r="107" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8708,10 +8720,10 @@
         <v>859</v>
       </c>
       <c r="P107" s="1" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="Q107" s="1" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
     </row>
     <row r="108" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8758,10 +8770,10 @@
         <v>859</v>
       </c>
       <c r="P108" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="Q108" s="1" t="s">
         <v>917</v>
-      </c>
-      <c r="Q108" s="1" t="s">
-        <v>919</v>
       </c>
     </row>
     <row r="109" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8808,10 +8820,10 @@
         <v>859</v>
       </c>
       <c r="P109" s="1" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="Q109" s="1" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
     </row>
     <row r="110" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8858,10 +8870,10 @@
         <v>859</v>
       </c>
       <c r="P110" s="1" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="Q110" s="1" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
     </row>
     <row r="111" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8908,10 +8920,10 @@
         <v>859</v>
       </c>
       <c r="P111" s="1" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="Q111" s="1" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
     </row>
     <row r="112" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8958,7 +8970,7 @@
         <v>859</v>
       </c>
       <c r="P112" s="1" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="Q112" s="1" t="s">
         <v>641</v>
@@ -9008,10 +9020,10 @@
         <v>859</v>
       </c>
       <c r="P113" s="1" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="Q113" s="1" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
     </row>
     <row r="114" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9058,10 +9070,10 @@
         <v>859</v>
       </c>
       <c r="P114" s="1" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="Q114" s="1" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
     </row>
     <row r="115" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9108,10 +9120,10 @@
         <v>859</v>
       </c>
       <c r="P115" s="1" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="Q115" s="1" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
     </row>
     <row r="116" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9158,7 +9170,7 @@
         <v>859</v>
       </c>
       <c r="Q116" s="1" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
     </row>
     <row r="117" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9205,10 +9217,10 @@
         <v>859</v>
       </c>
       <c r="P117" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="Q117" s="1" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
     </row>
     <row r="118" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9255,10 +9267,10 @@
         <v>859</v>
       </c>
       <c r="P118" s="1" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="Q118" s="1" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
@@ -9305,10 +9317,10 @@
         <v>856</v>
       </c>
       <c r="P119" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="Q119" s="3" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
glass et al 2019 extraction
</commit_message>
<xml_diff>
--- a/data extraction /lit search metadata /wos176_final.xlsx
+++ b/data extraction /lit search metadata /wos176_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /lit search metadata /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D275593-20C0-E940-8327-F12288754F97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6341623C-BD2A-BD44-A4BD-80BB61095344}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28700" yWindow="1880" windowWidth="23980" windowHeight="10600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1676" uniqueCount="939">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1677" uniqueCount="939">
   <si>
     <t>label</t>
   </si>
@@ -2636,9 +2636,6 @@
     <t>figure 2, 3</t>
   </si>
   <si>
-    <t xml:space="preserve">dig into use of PCA here </t>
-  </si>
-  <si>
     <t>figure 1</t>
   </si>
   <si>
@@ -2838,6 +2835,9 @@
   </si>
   <si>
     <t xml:space="preserve">no raw values, expected values for model employed </t>
+  </si>
+  <si>
+    <t>dig into use of PCA here, couldn't find sample size in this article</t>
   </si>
 </sst>
 </file>
@@ -3700,7 +3700,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A29" sqref="A29:XFD29"/>
+      <selection pane="bottomLeft" activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3758,7 +3758,7 @@
         <v>10</v>
       </c>
       <c r="R1" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -4672,7 +4672,7 @@
         <v>866</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="24" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4725,7 +4725,7 @@
         <v>866</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="25" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4778,7 +4778,7 @@
         <v>866</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="26" spans="1:18" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -4831,7 +4831,7 @@
         <v>866</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="27" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4884,7 +4884,7 @@
         <v>866</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
@@ -4990,7 +4990,7 @@
         <v>866</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
@@ -5096,7 +5096,10 @@
         <v>866</v>
       </c>
       <c r="Q31" t="s">
-        <v>871</v>
+        <v>938</v>
+      </c>
+      <c r="R31" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
@@ -5143,13 +5146,13 @@
         <v>856</v>
       </c>
       <c r="O32" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="P32" t="s">
         <v>866</v>
       </c>
       <c r="Q32" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
@@ -5196,13 +5199,13 @@
         <v>856</v>
       </c>
       <c r="O33" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="P33" t="s">
         <v>866</v>
       </c>
       <c r="Q33" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
@@ -5255,7 +5258,7 @@
         <v>866</v>
       </c>
       <c r="Q34" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="35" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5305,7 +5308,7 @@
         <v>866</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
@@ -5358,7 +5361,7 @@
         <v>866</v>
       </c>
       <c r="Q36" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="37" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5405,13 +5408,13 @@
         <v>856</v>
       </c>
       <c r="O37" s="2" t="s">
+        <v>879</v>
+      </c>
+      <c r="P37" s="2" t="s">
+        <v>881</v>
+      </c>
+      <c r="Q37" s="2" t="s">
         <v>880</v>
-      </c>
-      <c r="P37" s="2" t="s">
-        <v>882</v>
-      </c>
-      <c r="Q37" s="2" t="s">
-        <v>881</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
@@ -5458,13 +5461,13 @@
         <v>856</v>
       </c>
       <c r="O38" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="P38" t="s">
         <v>866</v>
       </c>
       <c r="Q38" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
@@ -5564,7 +5567,7 @@
         <v>866</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
@@ -5617,7 +5620,7 @@
         <v>866</v>
       </c>
       <c r="Q41" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.2">
@@ -5664,13 +5667,13 @@
         <v>859</v>
       </c>
       <c r="O42" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="P42" t="s">
         <v>866</v>
       </c>
       <c r="Q42" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="R42" t="s">
         <v>857</v>
@@ -5723,7 +5726,7 @@
         <v>866</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
@@ -5770,7 +5773,7 @@
         <v>856</v>
       </c>
       <c r="O44" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="P44" t="s">
         <v>866</v>
@@ -5870,13 +5873,13 @@
         <v>856</v>
       </c>
       <c r="O46" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="P46" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="Q46" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">
@@ -5923,13 +5926,13 @@
         <v>856</v>
       </c>
       <c r="O47" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="P47" t="s">
         <v>866</v>
       </c>
       <c r="Q47" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="48" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5979,7 +5982,7 @@
         <v>866</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
@@ -6026,7 +6029,7 @@
         <v>856</v>
       </c>
       <c r="O49" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="P49" t="s">
         <v>866</v>
@@ -6076,7 +6079,7 @@
         <v>856</v>
       </c>
       <c r="O50" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="P50" t="s">
         <v>866</v>
@@ -6126,13 +6129,13 @@
         <v>856</v>
       </c>
       <c r="O51" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="P51" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="Q51" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="52" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6179,7 +6182,7 @@
         <v>859</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
@@ -6226,7 +6229,7 @@
         <v>856</v>
       </c>
       <c r="O53" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="P53" t="s">
         <v>866</v>
@@ -6276,7 +6279,7 @@
         <v>859</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="55" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6323,7 +6326,7 @@
         <v>859</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
@@ -6370,13 +6373,13 @@
         <v>856</v>
       </c>
       <c r="O56" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="P56" t="s">
         <v>866</v>
       </c>
       <c r="Q56" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="57" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6423,7 +6426,7 @@
         <v>859</v>
       </c>
       <c r="Q57" s="1" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
@@ -6470,7 +6473,7 @@
         <v>856</v>
       </c>
       <c r="O58" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="P58" t="s">
         <v>866</v>
@@ -6521,13 +6524,13 @@
         <v>856</v>
       </c>
       <c r="O59" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="P59" t="s">
         <v>866</v>
       </c>
       <c r="Q59" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="60" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6574,7 +6577,7 @@
         <v>859</v>
       </c>
       <c r="Q60" s="1" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
@@ -6621,13 +6624,13 @@
         <v>856</v>
       </c>
       <c r="O61" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="P61" s="3" t="s">
         <v>866</v>
       </c>
       <c r="Q61" s="3" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="62" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6674,7 +6677,7 @@
         <v>859</v>
       </c>
       <c r="Q62" s="1" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
@@ -6721,7 +6724,7 @@
         <v>856</v>
       </c>
       <c r="O63" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="P63" s="3" t="s">
         <v>866</v>
@@ -6771,13 +6774,13 @@
         <v>856</v>
       </c>
       <c r="O64" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="P64" s="3" t="s">
         <v>866</v>
       </c>
       <c r="Q64" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
@@ -6824,7 +6827,7 @@
         <v>856</v>
       </c>
       <c r="O65" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="P65" s="3" t="s">
         <v>866</v>
@@ -6930,7 +6933,7 @@
         <v>866</v>
       </c>
       <c r="Q67" s="3" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="68" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6980,7 +6983,7 @@
         <v>866</v>
       </c>
       <c r="Q68" s="1" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="69" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7030,7 +7033,7 @@
         <v>866</v>
       </c>
       <c r="Q69" s="1" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="70" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7080,7 +7083,7 @@
         <v>866</v>
       </c>
       <c r="Q70" s="1" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="71" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7177,7 +7180,7 @@
         <v>866</v>
       </c>
       <c r="Q72" s="1" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="73" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7227,7 +7230,7 @@
         <v>866</v>
       </c>
       <c r="Q73" s="1" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="74" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7274,10 +7277,10 @@
         <v>859</v>
       </c>
       <c r="P74" s="1" t="s">
+        <v>911</v>
+      </c>
+      <c r="Q74" s="1" t="s">
         <v>912</v>
-      </c>
-      <c r="Q74" s="1" t="s">
-        <v>913</v>
       </c>
     </row>
     <row r="75" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -7529,10 +7532,10 @@
         <v>859</v>
       </c>
       <c r="P80" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="Q80" s="1" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="81" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8326,10 +8329,10 @@
         <v>859</v>
       </c>
       <c r="P99" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="Q99" s="1" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="100" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8423,10 +8426,10 @@
         <v>859</v>
       </c>
       <c r="P101" s="1" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="Q101" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="102" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8473,10 +8476,10 @@
         <v>859</v>
       </c>
       <c r="P102" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="Q102" s="1" t="s">
         <v>915</v>
-      </c>
-      <c r="Q102" s="1" t="s">
-        <v>916</v>
       </c>
     </row>
     <row r="103" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8523,10 +8526,10 @@
         <v>859</v>
       </c>
       <c r="P103" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="Q103" s="1" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="104" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8573,10 +8576,10 @@
         <v>859</v>
       </c>
       <c r="P104" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="Q104" s="1" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="105" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8623,10 +8626,10 @@
         <v>859</v>
       </c>
       <c r="P105" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="Q105" s="1" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="106" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8673,10 +8676,10 @@
         <v>859</v>
       </c>
       <c r="P106" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="Q106" s="1" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="107" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8723,10 +8726,10 @@
         <v>859</v>
       </c>
       <c r="P107" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="Q107" s="1" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="108" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8773,10 +8776,10 @@
         <v>859</v>
       </c>
       <c r="P108" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="Q108" s="1" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="109" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8823,10 +8826,10 @@
         <v>859</v>
       </c>
       <c r="P109" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="Q109" s="1" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="110" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8873,10 +8876,10 @@
         <v>859</v>
       </c>
       <c r="P110" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="Q110" s="1" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="111" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8923,10 +8926,10 @@
         <v>859</v>
       </c>
       <c r="P111" s="1" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="Q111" s="1" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="112" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8973,7 +8976,7 @@
         <v>859</v>
       </c>
       <c r="P112" s="1" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="Q112" s="1" t="s">
         <v>641</v>
@@ -9023,10 +9026,10 @@
         <v>859</v>
       </c>
       <c r="P113" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="Q113" s="1" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="114" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9073,10 +9076,10 @@
         <v>859</v>
       </c>
       <c r="P114" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="Q114" s="1" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="115" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9123,10 +9126,10 @@
         <v>859</v>
       </c>
       <c r="P115" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="Q115" s="1" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="116" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9173,7 +9176,7 @@
         <v>859</v>
       </c>
       <c r="Q116" s="1" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="117" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9220,10 +9223,10 @@
         <v>859</v>
       </c>
       <c r="P117" s="1" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="Q117" s="1" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="118" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9270,10 +9273,10 @@
         <v>859</v>
       </c>
       <c r="P118" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="Q118" s="1" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
@@ -9320,10 +9323,10 @@
         <v>856</v>
       </c>
       <c r="P119" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="Q119" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to extractable paper master list
</commit_message>
<xml_diff>
--- a/data extraction /lit search metadata /wos176_final.xlsx
+++ b/data extraction /lit search metadata /wos176_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /lit search metadata /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6341623C-BD2A-BD44-A4BD-80BB61095344}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBA9860-7618-4F4F-905A-8445465A1FA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28700" yWindow="1880" windowWidth="23980" windowHeight="10600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2642,9 +2642,6 @@
     <t>figure 1,2,3</t>
   </si>
   <si>
-    <t xml:space="preserve">not sure about the different life stages manipulated </t>
-  </si>
-  <si>
     <t>heatshock, not sure if it would be good extract this response value</t>
   </si>
   <si>
@@ -2838,6 +2835,9 @@
   </si>
   <si>
     <t>dig into use of PCA here, couldn't find sample size in this article</t>
+  </si>
+  <si>
+    <t>pulse press, acclimation experiment</t>
   </si>
 </sst>
 </file>
@@ -3699,8 +3699,8 @@
   <dimension ref="A1:R119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N18" sqref="N18"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3758,7 +3758,7 @@
         <v>10</v>
       </c>
       <c r="R1" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -4672,7 +4672,7 @@
         <v>866</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="24" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4725,7 +4725,7 @@
         <v>866</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="25" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4778,7 +4778,7 @@
         <v>866</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="26" spans="1:18" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -4831,7 +4831,7 @@
         <v>866</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="27" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4884,7 +4884,7 @@
         <v>866</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
@@ -4990,7 +4990,7 @@
         <v>866</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
@@ -5096,63 +5096,63 @@
         <v>866</v>
       </c>
       <c r="Q31" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="R31" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="32" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="1">
         <v>2016</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I32" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="J32" t="s">
-        <v>21</v>
-      </c>
-      <c r="K32" t="s">
+      <c r="J32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K32" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="L32" t="s">
-        <v>21</v>
-      </c>
-      <c r="M32" t="s">
+      <c r="L32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M32" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N32" t="s">
-        <v>856</v>
-      </c>
-      <c r="O32" t="s">
+      <c r="N32" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="O32" s="1" t="s">
         <v>872</v>
       </c>
-      <c r="P32" t="s">
+      <c r="P32" s="1" t="s">
         <v>866</v>
       </c>
-      <c r="Q32" t="s">
-        <v>873</v>
+      <c r="Q32" s="1" t="s">
+        <v>938</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
@@ -5199,13 +5199,13 @@
         <v>856</v>
       </c>
       <c r="O33" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="P33" t="s">
         <v>866</v>
       </c>
       <c r="Q33" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
@@ -5258,7 +5258,7 @@
         <v>866</v>
       </c>
       <c r="Q34" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="35" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5308,7 +5308,7 @@
         <v>866</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
@@ -5361,7 +5361,7 @@
         <v>866</v>
       </c>
       <c r="Q36" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="37" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5408,13 +5408,13 @@
         <v>856</v>
       </c>
       <c r="O37" s="2" t="s">
+        <v>878</v>
+      </c>
+      <c r="P37" s="2" t="s">
+        <v>880</v>
+      </c>
+      <c r="Q37" s="2" t="s">
         <v>879</v>
-      </c>
-      <c r="P37" s="2" t="s">
-        <v>881</v>
-      </c>
-      <c r="Q37" s="2" t="s">
-        <v>880</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
@@ -5461,13 +5461,13 @@
         <v>856</v>
       </c>
       <c r="O38" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="P38" t="s">
         <v>866</v>
       </c>
       <c r="Q38" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
@@ -5567,7 +5567,7 @@
         <v>866</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
@@ -5620,62 +5620,62 @@
         <v>866</v>
       </c>
       <c r="Q41" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="F42" s="1">
+        <v>2006</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="O42" s="1" t="s">
         <v>885</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>307</v>
-      </c>
-      <c r="B42" t="s">
-        <v>308</v>
-      </c>
-      <c r="C42" t="s">
-        <v>309</v>
-      </c>
-      <c r="D42" t="s">
-        <v>103</v>
-      </c>
-      <c r="E42" t="s">
-        <v>310</v>
-      </c>
-      <c r="F42">
-        <v>2006</v>
-      </c>
-      <c r="G42" t="s">
-        <v>311</v>
-      </c>
-      <c r="H42" t="s">
-        <v>106</v>
-      </c>
-      <c r="I42" t="s">
-        <v>312</v>
-      </c>
-      <c r="J42" t="s">
-        <v>21</v>
-      </c>
-      <c r="K42" t="s">
-        <v>313</v>
-      </c>
-      <c r="L42" t="s">
-        <v>21</v>
-      </c>
-      <c r="M42" t="s">
-        <v>23</v>
-      </c>
-      <c r="N42" t="s">
-        <v>859</v>
-      </c>
-      <c r="O42" t="s">
-        <v>886</v>
-      </c>
-      <c r="P42" t="s">
+      <c r="P42" s="1" t="s">
         <v>866</v>
       </c>
-      <c r="Q42" t="s">
-        <v>935</v>
-      </c>
-      <c r="R42" t="s">
+      <c r="Q42" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="R42" s="1" t="s">
         <v>857</v>
       </c>
     </row>
@@ -5726,7 +5726,7 @@
         <v>866</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
@@ -5773,7 +5773,7 @@
         <v>856</v>
       </c>
       <c r="O44" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="P44" t="s">
         <v>866</v>
@@ -5876,10 +5876,10 @@
         <v>871</v>
       </c>
       <c r="P46" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="Q46" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">
@@ -5932,7 +5932,7 @@
         <v>866</v>
       </c>
       <c r="Q47" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="48" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5982,7 +5982,7 @@
         <v>866</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
@@ -6029,7 +6029,7 @@
         <v>856</v>
       </c>
       <c r="O49" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="P49" t="s">
         <v>866</v>
@@ -6079,7 +6079,7 @@
         <v>856</v>
       </c>
       <c r="O50" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="P50" t="s">
         <v>866</v>
@@ -6129,13 +6129,13 @@
         <v>856</v>
       </c>
       <c r="O51" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="P51" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="Q51" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="52" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6182,7 +6182,7 @@
         <v>859</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
@@ -6229,7 +6229,7 @@
         <v>856</v>
       </c>
       <c r="O53" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="P53" t="s">
         <v>866</v>
@@ -6279,7 +6279,7 @@
         <v>859</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="55" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6326,7 +6326,7 @@
         <v>859</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
@@ -6379,7 +6379,7 @@
         <v>866</v>
       </c>
       <c r="Q56" s="3" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="57" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6426,7 +6426,7 @@
         <v>859</v>
       </c>
       <c r="Q57" s="1" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
@@ -6530,7 +6530,7 @@
         <v>866</v>
       </c>
       <c r="Q59" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="60" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6577,7 +6577,7 @@
         <v>859</v>
       </c>
       <c r="Q60" s="1" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
@@ -6630,7 +6630,7 @@
         <v>866</v>
       </c>
       <c r="Q61" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="62" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6677,7 +6677,7 @@
         <v>859</v>
       </c>
       <c r="Q62" s="1" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
@@ -6724,7 +6724,7 @@
         <v>856</v>
       </c>
       <c r="O63" s="3" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="P63" s="3" t="s">
         <v>866</v>
@@ -6780,7 +6780,7 @@
         <v>866</v>
       </c>
       <c r="Q64" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
@@ -6933,7 +6933,7 @@
         <v>866</v>
       </c>
       <c r="Q67" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="68" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6983,7 +6983,7 @@
         <v>866</v>
       </c>
       <c r="Q68" s="1" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="69" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7033,7 +7033,7 @@
         <v>866</v>
       </c>
       <c r="Q69" s="1" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="70" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7083,7 +7083,7 @@
         <v>866</v>
       </c>
       <c r="Q70" s="1" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="71" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7180,7 +7180,7 @@
         <v>866</v>
       </c>
       <c r="Q72" s="1" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="73" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7230,7 +7230,7 @@
         <v>866</v>
       </c>
       <c r="Q73" s="1" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="74" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7277,10 +7277,10 @@
         <v>859</v>
       </c>
       <c r="P74" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="Q74" s="1" t="s">
         <v>911</v>
-      </c>
-      <c r="Q74" s="1" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="75" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -7532,10 +7532,10 @@
         <v>859</v>
       </c>
       <c r="P80" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="Q80" s="1" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="81" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8329,10 +8329,10 @@
         <v>859</v>
       </c>
       <c r="P99" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="Q99" s="1" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="100" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8426,10 +8426,10 @@
         <v>859</v>
       </c>
       <c r="P101" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="Q101" s="1" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="102" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8476,10 +8476,10 @@
         <v>859</v>
       </c>
       <c r="P102" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="Q102" s="1" t="s">
         <v>914</v>
-      </c>
-      <c r="Q102" s="1" t="s">
-        <v>915</v>
       </c>
     </row>
     <row r="103" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8526,10 +8526,10 @@
         <v>859</v>
       </c>
       <c r="P103" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="Q103" s="1" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="104" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8576,10 +8576,10 @@
         <v>859</v>
       </c>
       <c r="P104" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="Q104" s="1" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="105" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8626,10 +8626,10 @@
         <v>859</v>
       </c>
       <c r="P105" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="Q105" s="1" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="106" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8676,10 +8676,10 @@
         <v>859</v>
       </c>
       <c r="P106" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="Q106" s="1" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="107" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8726,10 +8726,10 @@
         <v>859</v>
       </c>
       <c r="P107" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="Q107" s="1" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="108" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8776,10 +8776,10 @@
         <v>859</v>
       </c>
       <c r="P108" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="Q108" s="1" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="109" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8826,10 +8826,10 @@
         <v>859</v>
       </c>
       <c r="P109" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="Q109" s="1" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="110" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8876,10 +8876,10 @@
         <v>859</v>
       </c>
       <c r="P110" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="Q110" s="1" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="111" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8926,10 +8926,10 @@
         <v>859</v>
       </c>
       <c r="P111" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="Q111" s="1" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="112" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8976,7 +8976,7 @@
         <v>859</v>
       </c>
       <c r="P112" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="Q112" s="1" t="s">
         <v>641</v>
@@ -9026,10 +9026,10 @@
         <v>859</v>
       </c>
       <c r="P113" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="Q113" s="1" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="114" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9076,10 +9076,10 @@
         <v>859</v>
       </c>
       <c r="P114" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="Q114" s="1" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="115" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9126,10 +9126,10 @@
         <v>859</v>
       </c>
       <c r="P115" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="Q115" s="1" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="116" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9176,7 +9176,7 @@
         <v>859</v>
       </c>
       <c r="Q116" s="1" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="117" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9223,10 +9223,10 @@
         <v>859</v>
       </c>
       <c r="P117" s="1" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="Q117" s="1" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="118" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9273,10 +9273,10 @@
         <v>859</v>
       </c>
       <c r="P118" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="Q118" s="1" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
@@ -9323,10 +9323,10 @@
         <v>856</v>
       </c>
       <c r="P119" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="Q119" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
committing to avoid merge conflict
</commit_message>
<xml_diff>
--- a/data extraction /lit search metadata /wos176_final.xlsx
+++ b/data extraction /lit search metadata /wos176_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /lit search metadata /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5BD3DE-EC22-C548-80E9-9CAB4FCBD4D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3002A2E-1C88-4E42-87D1-87183B719B71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28700" yWindow="1880" windowWidth="23980" windowHeight="10600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="939">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1679" uniqueCount="939">
   <si>
     <t>label</t>
   </si>
@@ -2642,9 +2642,6 @@
     <t>figure 1,2,3</t>
   </si>
   <si>
-    <t>heatshock, not sure if it would be good extract this response value</t>
-  </si>
-  <si>
     <t>table 1, figure 2, 3, 5</t>
   </si>
   <si>
@@ -2837,7 +2834,10 @@
     <t>pulse press, acclimation experiment</t>
   </si>
   <si>
-    <t>looks like the responses were generated in different temperature treatments from their constant/flux rearing conditions (return for acclimation/pulse press experiments; not sure about sample sizes for table 1 (check out results referencing the results of table 1)</t>
+    <t>heatshock, return for pulse press experiments work; missing sample size for current extraction</t>
+  </si>
+  <si>
+    <t>might need to return to get actual irradiances for UV treatments (they manipulated both temperature and irradiance in these experiments)</t>
   </si>
 </sst>
 </file>
@@ -3699,8 +3699,8 @@
   <dimension ref="A1:R119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q34" sqref="Q34"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S39" sqref="S39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3758,7 +3758,7 @@
         <v>10</v>
       </c>
       <c r="R1" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -4672,7 +4672,7 @@
         <v>866</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="24" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4725,7 +4725,7 @@
         <v>866</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="25" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4778,7 +4778,7 @@
         <v>866</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="26" spans="1:18" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -4831,7 +4831,7 @@
         <v>866</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="27" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4884,7 +4884,7 @@
         <v>866</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
@@ -4990,7 +4990,7 @@
         <v>866</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
@@ -5096,7 +5096,7 @@
         <v>866</v>
       </c>
       <c r="Q31" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="R31" t="s">
         <v>23</v>
@@ -5152,7 +5152,7 @@
         <v>866</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
@@ -5199,13 +5199,13 @@
         <v>856</v>
       </c>
       <c r="O33" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="P33" t="s">
         <v>866</v>
       </c>
       <c r="Q33" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="R33" t="s">
         <v>23</v>
@@ -5261,7 +5261,10 @@
         <v>866</v>
       </c>
       <c r="Q34" t="s">
-        <v>873</v>
+        <v>938</v>
+      </c>
+      <c r="R34" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5311,7 +5314,7 @@
         <v>866</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
@@ -5364,7 +5367,7 @@
         <v>866</v>
       </c>
       <c r="Q36" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="37" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5411,13 +5414,13 @@
         <v>856</v>
       </c>
       <c r="O37" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="P37" s="2" t="s">
+        <v>878</v>
+      </c>
+      <c r="Q37" s="2" t="s">
         <v>877</v>
-      </c>
-      <c r="P37" s="2" t="s">
-        <v>879</v>
-      </c>
-      <c r="Q37" s="2" t="s">
-        <v>878</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
@@ -5464,13 +5467,13 @@
         <v>856</v>
       </c>
       <c r="O38" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="P38" t="s">
         <v>866</v>
       </c>
       <c r="Q38" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
@@ -5570,7 +5573,7 @@
         <v>866</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
@@ -5623,7 +5626,7 @@
         <v>866</v>
       </c>
       <c r="Q41" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="42" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5670,13 +5673,13 @@
         <v>859</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="P42" s="1" t="s">
         <v>866</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="R42" s="1" t="s">
         <v>857</v>
@@ -5729,7 +5732,7 @@
         <v>866</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
@@ -5776,7 +5779,7 @@
         <v>856</v>
       </c>
       <c r="O44" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="P44" t="s">
         <v>866</v>
@@ -5879,10 +5882,10 @@
         <v>871</v>
       </c>
       <c r="P46" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="Q46" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">
@@ -5935,7 +5938,7 @@
         <v>866</v>
       </c>
       <c r="Q47" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="48" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5985,7 +5988,7 @@
         <v>866</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
@@ -6032,7 +6035,7 @@
         <v>856</v>
       </c>
       <c r="O49" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="P49" t="s">
         <v>866</v>
@@ -6082,7 +6085,7 @@
         <v>856</v>
       </c>
       <c r="O50" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="P50" t="s">
         <v>866</v>
@@ -6132,13 +6135,13 @@
         <v>856</v>
       </c>
       <c r="O51" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="P51" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="Q51" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="52" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6185,7 +6188,7 @@
         <v>859</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
@@ -6232,7 +6235,7 @@
         <v>856</v>
       </c>
       <c r="O53" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="P53" t="s">
         <v>866</v>
@@ -6282,7 +6285,7 @@
         <v>859</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="55" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6329,7 +6332,7 @@
         <v>859</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
@@ -6382,7 +6385,7 @@
         <v>866</v>
       </c>
       <c r="Q56" s="3" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="57" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6429,7 +6432,7 @@
         <v>859</v>
       </c>
       <c r="Q57" s="1" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
@@ -6533,7 +6536,7 @@
         <v>866</v>
       </c>
       <c r="Q59" s="3" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="60" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6580,7 +6583,7 @@
         <v>859</v>
       </c>
       <c r="Q60" s="1" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
@@ -6633,7 +6636,7 @@
         <v>866</v>
       </c>
       <c r="Q61" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="62" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6680,7 +6683,7 @@
         <v>859</v>
       </c>
       <c r="Q62" s="1" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
@@ -6727,7 +6730,7 @@
         <v>856</v>
       </c>
       <c r="O63" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="P63" s="3" t="s">
         <v>866</v>
@@ -6783,7 +6786,7 @@
         <v>866</v>
       </c>
       <c r="Q64" s="3" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
@@ -6936,7 +6939,7 @@
         <v>866</v>
       </c>
       <c r="Q67" s="3" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="68" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6986,7 +6989,7 @@
         <v>866</v>
       </c>
       <c r="Q68" s="1" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="69" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7036,7 +7039,7 @@
         <v>866</v>
       </c>
       <c r="Q69" s="1" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="70" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7086,7 +7089,7 @@
         <v>866</v>
       </c>
       <c r="Q70" s="1" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="71" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7183,7 +7186,7 @@
         <v>866</v>
       </c>
       <c r="Q72" s="1" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="73" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7233,7 +7236,7 @@
         <v>866</v>
       </c>
       <c r="Q73" s="1" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="74" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7280,10 +7283,10 @@
         <v>859</v>
       </c>
       <c r="P74" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="Q74" s="1" t="s">
         <v>909</v>
-      </c>
-      <c r="Q74" s="1" t="s">
-        <v>910</v>
       </c>
     </row>
     <row r="75" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -7535,10 +7538,10 @@
         <v>859</v>
       </c>
       <c r="P80" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="Q80" s="1" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="81" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8332,10 +8335,10 @@
         <v>859</v>
       </c>
       <c r="P99" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="Q99" s="1" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="100" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8429,10 +8432,10 @@
         <v>859</v>
       </c>
       <c r="P101" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="Q101" s="1" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="102" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8479,10 +8482,10 @@
         <v>859</v>
       </c>
       <c r="P102" s="1" t="s">
+        <v>911</v>
+      </c>
+      <c r="Q102" s="1" t="s">
         <v>912</v>
-      </c>
-      <c r="Q102" s="1" t="s">
-        <v>913</v>
       </c>
     </row>
     <row r="103" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8529,10 +8532,10 @@
         <v>859</v>
       </c>
       <c r="P103" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="Q103" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="104" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8579,10 +8582,10 @@
         <v>859</v>
       </c>
       <c r="P104" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="Q104" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="105" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8629,10 +8632,10 @@
         <v>859</v>
       </c>
       <c r="P105" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="Q105" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="106" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8679,10 +8682,10 @@
         <v>859</v>
       </c>
       <c r="P106" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="Q106" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="107" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8729,10 +8732,10 @@
         <v>859</v>
       </c>
       <c r="P107" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="Q107" s="1" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="108" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8779,10 +8782,10 @@
         <v>859</v>
       </c>
       <c r="P108" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="Q108" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="109" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8829,10 +8832,10 @@
         <v>859</v>
       </c>
       <c r="P109" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="Q109" s="1" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="110" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8879,10 +8882,10 @@
         <v>859</v>
       </c>
       <c r="P110" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="Q110" s="1" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="111" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8929,10 +8932,10 @@
         <v>859</v>
       </c>
       <c r="P111" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="Q111" s="1" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="112" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8979,7 +8982,7 @@
         <v>859</v>
       </c>
       <c r="P112" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="Q112" s="1" t="s">
         <v>641</v>
@@ -9029,10 +9032,10 @@
         <v>859</v>
       </c>
       <c r="P113" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="Q113" s="1" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="114" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9079,10 +9082,10 @@
         <v>859</v>
       </c>
       <c r="P114" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="Q114" s="1" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="115" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9129,10 +9132,10 @@
         <v>859</v>
       </c>
       <c r="P115" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="Q115" s="1" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="116" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9179,7 +9182,7 @@
         <v>859</v>
       </c>
       <c r="Q116" s="1" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="117" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9226,10 +9229,10 @@
         <v>859</v>
       </c>
       <c r="P117" s="1" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="Q117" s="1" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="118" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9276,10 +9279,10 @@
         <v>859</v>
       </c>
       <c r="P118" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="Q118" s="1" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
@@ -9326,10 +9329,10 @@
         <v>856</v>
       </c>
       <c r="P119" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="Q119" s="3" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rolandi et al 2018 extraction
</commit_message>
<xml_diff>
--- a/data extraction /lit search metadata /wos176_final.xlsx
+++ b/data extraction /lit search metadata /wos176_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /lit search metadata /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DCED27-E923-8D49-8C8C-ED51402CEA8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCB5D4E-01C2-1C45-BCCF-13C55955CBD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28700" yWindow="1880" windowWidth="23980" windowHeight="10600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="7400" windowWidth="23980" windowHeight="10600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wos176_final" sheetId="1" r:id="rId1"/>
@@ -2651,15 +2651,9 @@
     <t xml:space="preserve">figure 2 </t>
   </si>
   <si>
-    <t xml:space="preserve">other graphs may provided good info for intro and thinking about the color of environmental noise </t>
-  </si>
-  <si>
     <t>population</t>
   </si>
   <si>
-    <t>data available in figshare</t>
-  </si>
-  <si>
     <t>figure 2, 4</t>
   </si>
   <si>
@@ -2838,6 +2832,12 @@
   </si>
   <si>
     <t xml:space="preserve">predictable and unpredictable variability; extracted all of figure 2 except for 2b and 2d--return to this for pulse press or acclimation assay experiments for cold exposure recovery etc </t>
+  </si>
+  <si>
+    <t>other graphs may provided good info for intro and thinking about the color of environmental noise ; excluded because main figure for data did not have error reported and none of the other figures appear to be metrics that we could include for analysis with other studies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data available in figshare--not usable without errors; extracted data from figure but can't locate sample size </t>
   </si>
 </sst>
 </file>
@@ -2980,7 +2980,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3166,12 +3166,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -3333,10 +3327,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3699,7 +3692,7 @@
   <dimension ref="A1:R119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Q38" sqref="Q38"/>
     </sheetView>
   </sheetViews>
@@ -3758,7 +3751,7 @@
         <v>10</v>
       </c>
       <c r="R1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -4672,7 +4665,7 @@
         <v>866</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
     </row>
     <row r="24" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4725,7 +4718,7 @@
         <v>866</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
     </row>
     <row r="25" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4778,7 +4771,7 @@
         <v>866</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="26" spans="1:18" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -4831,7 +4824,7 @@
         <v>866</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
     </row>
     <row r="27" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4884,7 +4877,7 @@
         <v>866</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
@@ -4990,7 +4983,7 @@
         <v>866</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
@@ -5096,7 +5089,7 @@
         <v>866</v>
       </c>
       <c r="Q31" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="R31" t="s">
         <v>23</v>
@@ -5152,7 +5145,7 @@
         <v>866</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
@@ -5205,7 +5198,7 @@
         <v>866</v>
       </c>
       <c r="Q33" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="R33" t="s">
         <v>23</v>
@@ -5261,7 +5254,7 @@
         <v>866</v>
       </c>
       <c r="Q34" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="R34" t="s">
         <v>23</v>
@@ -5367,63 +5360,63 @@
         <v>866</v>
       </c>
       <c r="Q36" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="R36" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+    <row r="37" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E37" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F37" s="1">
         <v>2000</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G37" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="H37" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I37" s="2" t="s">
+      <c r="I37" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="J37" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K37" s="2" t="s">
+      <c r="J37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K37" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="L37" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M37" s="2" t="s">
+      <c r="L37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M37" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N37" s="2" t="s">
-        <v>856</v>
-      </c>
-      <c r="O37" s="2" t="s">
+      <c r="N37" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="O37" s="1" t="s">
         <v>875</v>
       </c>
-      <c r="P37" s="2" t="s">
-        <v>877</v>
-      </c>
-      <c r="Q37" s="2" t="s">
+      <c r="P37" s="1" t="s">
         <v>876</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>937</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
@@ -5470,13 +5463,13 @@
         <v>856</v>
       </c>
       <c r="O38" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="P38" t="s">
         <v>866</v>
       </c>
       <c r="Q38" t="s">
-        <v>878</v>
+        <v>938</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
@@ -5576,7 +5569,7 @@
         <v>866</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
@@ -5629,7 +5622,7 @@
         <v>866</v>
       </c>
       <c r="Q41" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
     </row>
     <row r="42" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5676,13 +5669,13 @@
         <v>859</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="P42" s="1" t="s">
         <v>866</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="R42" s="1" t="s">
         <v>857</v>
@@ -5735,7 +5728,7 @@
         <v>866</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
@@ -5782,7 +5775,7 @@
         <v>856</v>
       </c>
       <c r="O44" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="P44" t="s">
         <v>866</v>
@@ -5885,10 +5878,10 @@
         <v>871</v>
       </c>
       <c r="P46" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="Q46" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">
@@ -5941,7 +5934,7 @@
         <v>866</v>
       </c>
       <c r="Q47" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
     </row>
     <row r="48" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5991,7 +5984,7 @@
         <v>866</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
@@ -6038,7 +6031,7 @@
         <v>856</v>
       </c>
       <c r="O49" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="P49" t="s">
         <v>866</v>
@@ -6088,7 +6081,7 @@
         <v>856</v>
       </c>
       <c r="O50" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="P50" t="s">
         <v>866</v>
@@ -6138,13 +6131,13 @@
         <v>856</v>
       </c>
       <c r="O51" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="P51" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="Q51" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
     </row>
     <row r="52" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6191,7 +6184,7 @@
         <v>859</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
@@ -6238,7 +6231,7 @@
         <v>856</v>
       </c>
       <c r="O53" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="P53" t="s">
         <v>866</v>
@@ -6288,7 +6281,7 @@
         <v>859</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
     </row>
     <row r="55" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6335,7 +6328,7 @@
         <v>859</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
@@ -6378,17 +6371,17 @@
       <c r="M56" t="s">
         <v>856</v>
       </c>
-      <c r="N56" s="3" t="s">
+      <c r="N56" s="2" t="s">
         <v>856</v>
       </c>
-      <c r="O56" s="3" t="s">
+      <c r="O56" s="2" t="s">
         <v>871</v>
       </c>
       <c r="P56" t="s">
         <v>866</v>
       </c>
-      <c r="Q56" s="3" t="s">
-        <v>893</v>
+      <c r="Q56" s="2" t="s">
+        <v>891</v>
       </c>
     </row>
     <row r="57" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6435,7 +6428,7 @@
         <v>859</v>
       </c>
       <c r="Q57" s="1" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
@@ -6478,7 +6471,7 @@
       <c r="M58" t="s">
         <v>856</v>
       </c>
-      <c r="N58" s="3" t="s">
+      <c r="N58" s="2" t="s">
         <v>856</v>
       </c>
       <c r="O58" t="s">
@@ -6487,7 +6480,7 @@
       <c r="P58" t="s">
         <v>866</v>
       </c>
-      <c r="Q58" s="3"/>
+      <c r="Q58" s="2"/>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
@@ -6529,7 +6522,7 @@
       <c r="M59" t="s">
         <v>856</v>
       </c>
-      <c r="N59" s="3" t="s">
+      <c r="N59" s="2" t="s">
         <v>856</v>
       </c>
       <c r="O59" t="s">
@@ -6538,8 +6531,8 @@
       <c r="P59" t="s">
         <v>866</v>
       </c>
-      <c r="Q59" s="3" t="s">
-        <v>895</v>
+      <c r="Q59" s="2" t="s">
+        <v>893</v>
       </c>
     </row>
     <row r="60" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6586,7 +6579,7 @@
         <v>859</v>
       </c>
       <c r="Q60" s="1" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
@@ -6629,17 +6622,17 @@
       <c r="M61" t="s">
         <v>856</v>
       </c>
-      <c r="N61" s="3" t="s">
+      <c r="N61" s="2" t="s">
         <v>856</v>
       </c>
-      <c r="O61" s="3" t="s">
+      <c r="O61" s="2" t="s">
         <v>871</v>
       </c>
-      <c r="P61" s="3" t="s">
+      <c r="P61" s="2" t="s">
         <v>866</v>
       </c>
-      <c r="Q61" s="3" t="s">
-        <v>897</v>
+      <c r="Q61" s="2" t="s">
+        <v>895</v>
       </c>
     </row>
     <row r="62" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6686,7 +6679,7 @@
         <v>859</v>
       </c>
       <c r="Q62" s="1" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
@@ -6729,13 +6722,13 @@
       <c r="M63" t="s">
         <v>23</v>
       </c>
-      <c r="N63" s="3" t="s">
+      <c r="N63" s="2" t="s">
         <v>856</v>
       </c>
-      <c r="O63" s="3" t="s">
-        <v>899</v>
-      </c>
-      <c r="P63" s="3" t="s">
+      <c r="O63" s="2" t="s">
+        <v>897</v>
+      </c>
+      <c r="P63" s="2" t="s">
         <v>866</v>
       </c>
     </row>
@@ -6779,17 +6772,17 @@
       <c r="M64" t="s">
         <v>23</v>
       </c>
-      <c r="N64" s="3" t="s">
+      <c r="N64" s="2" t="s">
         <v>856</v>
       </c>
-      <c r="O64" s="3" t="s">
+      <c r="O64" s="2" t="s">
         <v>871</v>
       </c>
-      <c r="P64" s="3" t="s">
+      <c r="P64" s="2" t="s">
         <v>866</v>
       </c>
-      <c r="Q64" s="3" t="s">
-        <v>900</v>
+      <c r="Q64" s="2" t="s">
+        <v>898</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
@@ -6832,13 +6825,13 @@
       <c r="M65" t="s">
         <v>23</v>
       </c>
-      <c r="N65" s="3" t="s">
+      <c r="N65" s="2" t="s">
         <v>856</v>
       </c>
-      <c r="O65" s="3" t="s">
+      <c r="O65" s="2" t="s">
         <v>871</v>
       </c>
-      <c r="P65" s="3" t="s">
+      <c r="P65" s="2" t="s">
         <v>866</v>
       </c>
     </row>
@@ -6882,13 +6875,13 @@
       <c r="M66" t="s">
         <v>23</v>
       </c>
-      <c r="N66" s="3" t="s">
+      <c r="N66" s="2" t="s">
         <v>856</v>
       </c>
-      <c r="O66" s="3" t="s">
+      <c r="O66" s="2" t="s">
         <v>870</v>
       </c>
-      <c r="P66" s="3" t="s">
+      <c r="P66" s="2" t="s">
         <v>866</v>
       </c>
     </row>
@@ -6932,17 +6925,17 @@
       <c r="M67" t="s">
         <v>23</v>
       </c>
-      <c r="N67" s="3" t="s">
+      <c r="N67" s="2" t="s">
         <v>856</v>
       </c>
-      <c r="O67" s="3" t="s">
+      <c r="O67" s="2" t="s">
         <v>867</v>
       </c>
-      <c r="P67" s="3" t="s">
+      <c r="P67" s="2" t="s">
         <v>866</v>
       </c>
-      <c r="Q67" s="3" t="s">
-        <v>901</v>
+      <c r="Q67" s="2" t="s">
+        <v>899</v>
       </c>
     </row>
     <row r="68" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6992,7 +6985,7 @@
         <v>866</v>
       </c>
       <c r="Q68" s="1" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
     </row>
     <row r="69" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7042,7 +7035,7 @@
         <v>866</v>
       </c>
       <c r="Q69" s="1" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
     </row>
     <row r="70" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7092,7 +7085,7 @@
         <v>866</v>
       </c>
       <c r="Q70" s="1" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
     </row>
     <row r="71" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7189,10 +7182,10 @@
         <v>866</v>
       </c>
       <c r="Q72" s="1" t="s">
-        <v>905</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>514</v>
       </c>
@@ -7223,7 +7216,7 @@
       <c r="J73" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K73" s="4" t="s">
+      <c r="K73" s="3" t="s">
         <v>520</v>
       </c>
       <c r="L73" s="1" t="s">
@@ -7239,7 +7232,7 @@
         <v>866</v>
       </c>
       <c r="Q73" s="1" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
     </row>
     <row r="74" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7286,50 +7279,50 @@
         <v>859</v>
       </c>
       <c r="P74" s="1" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="Q74" s="1" t="s">
-        <v>908</v>
-      </c>
-    </row>
-    <row r="75" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="3" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="C75" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="D75" s="3" t="s">
+      <c r="D75" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="E75" s="3" t="s">
+      <c r="E75" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="F75" s="3">
+      <c r="F75" s="2">
         <v>2018</v>
       </c>
-      <c r="G75" s="3" t="s">
+      <c r="G75" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="H75" s="3" t="s">
+      <c r="H75" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="I75" s="3" t="s">
+      <c r="I75" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="J75" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K75" s="3" t="s">
+      <c r="J75" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K75" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="L75" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M75" s="3" t="s">
+      <c r="L75" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M75" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -7541,10 +7534,10 @@
         <v>859</v>
       </c>
       <c r="P80" s="1" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="Q80" s="1" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
     </row>
     <row r="81" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8338,10 +8331,10 @@
         <v>859</v>
       </c>
       <c r="P99" s="1" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="Q99" s="1" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
     </row>
     <row r="100" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8435,10 +8428,10 @@
         <v>859</v>
       </c>
       <c r="P101" s="1" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="Q101" s="1" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
     </row>
     <row r="102" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8485,10 +8478,10 @@
         <v>859</v>
       </c>
       <c r="P102" s="1" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="Q102" s="1" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
     </row>
     <row r="103" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8535,10 +8528,10 @@
         <v>859</v>
       </c>
       <c r="P103" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="Q103" s="1" t="s">
         <v>910</v>
-      </c>
-      <c r="Q103" s="1" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="104" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8585,10 +8578,10 @@
         <v>859</v>
       </c>
       <c r="P104" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="Q104" s="1" t="s">
         <v>910</v>
-      </c>
-      <c r="Q104" s="1" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="105" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8635,10 +8628,10 @@
         <v>859</v>
       </c>
       <c r="P105" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="Q105" s="1" t="s">
         <v>910</v>
-      </c>
-      <c r="Q105" s="1" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="106" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8685,10 +8678,10 @@
         <v>859</v>
       </c>
       <c r="P106" s="1" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="Q106" s="1" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
     </row>
     <row r="107" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8735,10 +8728,10 @@
         <v>859</v>
       </c>
       <c r="P107" s="1" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="Q107" s="1" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="108" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8785,10 +8778,10 @@
         <v>859</v>
       </c>
       <c r="P108" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="Q108" s="1" t="s">
         <v>910</v>
-      </c>
-      <c r="Q108" s="1" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="109" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8835,10 +8828,10 @@
         <v>859</v>
       </c>
       <c r="P109" s="1" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="Q109" s="1" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
     </row>
     <row r="110" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8885,10 +8878,10 @@
         <v>859</v>
       </c>
       <c r="P110" s="1" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="Q110" s="1" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="111" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8935,10 +8928,10 @@
         <v>859</v>
       </c>
       <c r="P111" s="1" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="Q111" s="1" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
     </row>
     <row r="112" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8985,7 +8978,7 @@
         <v>859</v>
       </c>
       <c r="P112" s="1" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="Q112" s="1" t="s">
         <v>641</v>
@@ -9035,10 +9028,10 @@
         <v>859</v>
       </c>
       <c r="P113" s="1" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="Q113" s="1" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="114" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9085,10 +9078,10 @@
         <v>859</v>
       </c>
       <c r="P114" s="1" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="Q114" s="1" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
     </row>
     <row r="115" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9135,10 +9128,10 @@
         <v>859</v>
       </c>
       <c r="P115" s="1" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="Q115" s="1" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
     </row>
     <row r="116" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9185,7 +9178,7 @@
         <v>859</v>
       </c>
       <c r="Q116" s="1" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
     </row>
     <row r="117" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9232,10 +9225,10 @@
         <v>859</v>
       </c>
       <c r="P117" s="1" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="Q117" s="1" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
     </row>
     <row r="118" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9282,10 +9275,10 @@
         <v>859</v>
       </c>
       <c r="P118" s="1" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="Q118" s="1" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
@@ -9328,14 +9321,14 @@
       <c r="M119" t="s">
         <v>856</v>
       </c>
-      <c r="N119" s="3" t="s">
+      <c r="N119" s="2" t="s">
         <v>856</v>
       </c>
       <c r="P119" t="s">
-        <v>910</v>
-      </c>
-      <c r="Q119" s="3" t="s">
-        <v>924</v>
+        <v>908</v>
+      </c>
+      <c r="Q119" s="2" t="s">
+        <v>922</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
triedel et al extraction updates
</commit_message>
<xml_diff>
--- a/data extraction /lit search metadata /wos176_final.xlsx
+++ b/data extraction /lit search metadata /wos176_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /lit search metadata /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195CC96E-0990-4248-A668-2EA1940C16CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA55029-67F5-4343-AF92-FAED409619A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2460" yWindow="460" windowWidth="23980" windowHeight="11900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1699" uniqueCount="948">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1700" uniqueCount="948">
   <si>
     <t>label</t>
   </si>
@@ -2678,15 +2678,9 @@
     <t>not sure about this study, it doesn't appear to have a constant treatment, only typical diurnal pattern with more extreme minima…</t>
   </si>
   <si>
-    <t xml:space="preserve">doesn't appear to have a no variation treatment </t>
-  </si>
-  <si>
     <t>transcriptome differences?</t>
   </si>
   <si>
-    <t xml:space="preserve">incubation in flux temps </t>
-  </si>
-  <si>
     <t>differentially expressed genes and PCA, data doesn't look extractable</t>
   </si>
   <si>
@@ -2849,22 +2843,28 @@
     <t>not sure about the f1 and f2 treatments features exposure to ambient temps? (eventhough they have the mean and range recorded)</t>
   </si>
   <si>
-    <t xml:space="preserve">cold acclimation data featured, unclear whether fluctuating and constant treatments can be extracted here </t>
-  </si>
-  <si>
     <t xml:space="preserve">unclear whther this should be considered multiple exposure or cold exposure--inclear whether there is a constant treatment to extract data frome </t>
   </si>
   <si>
     <t xml:space="preserve">return for cold exposure in figure 2 and figure 1; not sure how usable data for big met analysis is </t>
   </si>
   <si>
-    <t>didn't extract second fluctuating temperature treatment, extracted data from second table because corresponding species were explicitly labeled. Assumed sample size of 125 based on methods?</t>
-  </si>
-  <si>
     <t>doesn't appear to be extractable, has 95% CI in table 1+2, data available in dryad doesn't have error listed?</t>
   </si>
   <si>
     <t>cellular, parasite host relationship;  etxracted figure 1 and 2, not sure about sample size (listed 3 replicates randomly selected per treatment to anayze so assumed sample size of 3)</t>
+  </si>
+  <si>
+    <t>doesn't appear to have a no cnstant treatment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> extracted data from second table because corresponding species were explicitly labeled. Assumed sample size of 125- based on methods; upon looking at the methods, the upper table appears to be a daily calculation whereas the bottom calculation appears to be a total. just extracted the second table, extracted both fluctuating treatments and coded as ramping </t>
+  </si>
+  <si>
+    <t>cold acclimation data featured, unclear whether fluctuating and constant treatments can be extracted here ; no error reported for fluctuating treatment, only sample size?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incubation in flux temps,  extracted figure 2a for constant vs flux treatment. Extracted the x and y values as separate rows </t>
   </si>
 </sst>
 </file>
@@ -3719,8 +3719,8 @@
   <dimension ref="A1:R119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A119" sqref="A119:XFD119"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R50" sqref="R50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3778,7 +3778,7 @@
         <v>10</v>
       </c>
       <c r="R1" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -4692,7 +4692,7 @@
         <v>866</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
     </row>
     <row r="24" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4745,7 +4745,7 @@
         <v>866</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
     </row>
     <row r="25" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4798,7 +4798,7 @@
         <v>866</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
     </row>
     <row r="26" spans="1:18" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -4851,7 +4851,7 @@
         <v>866</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
     </row>
     <row r="27" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -4904,7 +4904,7 @@
         <v>866</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
@@ -5010,7 +5010,7 @@
         <v>866</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
@@ -5116,7 +5116,7 @@
         <v>866</v>
       </c>
       <c r="Q31" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="R31" t="s">
         <v>23</v>
@@ -5172,7 +5172,7 @@
         <v>866</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
@@ -5225,7 +5225,7 @@
         <v>866</v>
       </c>
       <c r="Q33" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="R33" t="s">
         <v>23</v>
@@ -5281,7 +5281,7 @@
         <v>866</v>
       </c>
       <c r="Q34" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="R34" t="s">
         <v>23</v>
@@ -5387,7 +5387,7 @@
         <v>866</v>
       </c>
       <c r="Q36" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="R36" t="s">
         <v>23</v>
@@ -5443,7 +5443,7 @@
         <v>876</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
@@ -5496,7 +5496,7 @@
         <v>866</v>
       </c>
       <c r="Q38" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="R38" t="s">
         <v>23</v>
@@ -5552,7 +5552,7 @@
         <v>866</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="R39" s="2" t="s">
         <v>23</v>
@@ -5658,7 +5658,7 @@
         <v>866</v>
       </c>
       <c r="Q41" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="R41" s="2" t="s">
         <v>23</v>
@@ -5714,7 +5714,7 @@
         <v>866</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="R42" s="1" t="s">
         <v>857</v>
@@ -5876,7 +5876,7 @@
         <v>866</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="46" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5929,7 +5929,7 @@
         <v>876</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
     </row>
     <row r="47" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5982,7 +5982,7 @@
         <v>866</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
     </row>
     <row r="48" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6138,7 +6138,7 @@
         <v>866</v>
       </c>
       <c r="Q50" s="2" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="R50" s="2" t="s">
         <v>23</v>
@@ -6194,7 +6194,7 @@
         <v>876</v>
       </c>
       <c r="Q51" t="s">
-        <v>947</v>
+        <v>943</v>
       </c>
       <c r="R51" t="s">
         <v>23</v>
@@ -6247,57 +6247,57 @@
         <v>884</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="53" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="1">
         <v>2014</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G53" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H53" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="I53" t="s">
+      <c r="I53" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="J53" t="s">
-        <v>21</v>
-      </c>
-      <c r="K53" t="s">
+      <c r="J53" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K53" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="L53" t="s">
-        <v>21</v>
-      </c>
-      <c r="M53" t="s">
+      <c r="L53" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M53" s="1" t="s">
         <v>856</v>
       </c>
-      <c r="N53" t="s">
+      <c r="N53" s="1" t="s">
         <v>856</v>
       </c>
-      <c r="O53" t="s">
+      <c r="O53" s="1" t="s">
         <v>882</v>
       </c>
-      <c r="P53" t="s">
+      <c r="P53" s="1" t="s">
         <v>866</v>
       </c>
-      <c r="Q53" t="s">
-        <v>942</v>
+      <c r="Q53" s="1" t="s">
+        <v>946</v>
       </c>
     </row>
     <row r="54" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6344,7 +6344,7 @@
         <v>859</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>885</v>
+        <v>944</v>
       </c>
     </row>
     <row r="55" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6391,7 +6391,7 @@
         <v>859</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.2">
@@ -6444,7 +6444,10 @@
         <v>866</v>
       </c>
       <c r="Q56" s="2" t="s">
-        <v>887</v>
+        <v>947</v>
+      </c>
+      <c r="R56" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="57" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6491,7 +6494,7 @@
         <v>859</v>
       </c>
       <c r="Q57" s="1" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.2">
@@ -6544,7 +6547,7 @@
         <v>866</v>
       </c>
       <c r="Q58" s="2" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
     </row>
     <row r="59" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6597,7 +6600,7 @@
         <v>866</v>
       </c>
       <c r="Q59" s="1" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
     </row>
     <row r="60" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6644,7 +6647,7 @@
         <v>859</v>
       </c>
       <c r="Q60" s="1" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
     </row>
     <row r="61" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6697,7 +6700,7 @@
         <v>866</v>
       </c>
       <c r="Q61" s="1" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
     </row>
     <row r="62" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6744,7 +6747,7 @@
         <v>859</v>
       </c>
       <c r="Q62" s="1" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.2">
@@ -6791,13 +6794,13 @@
         <v>856</v>
       </c>
       <c r="O63" s="2" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="P63" s="2" t="s">
         <v>866</v>
       </c>
       <c r="Q63" s="2" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="R63" s="2" t="s">
         <v>23</v>
@@ -6853,7 +6856,7 @@
         <v>866</v>
       </c>
       <c r="Q64" s="2" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="R64" s="2" t="s">
         <v>23</v>
@@ -6909,7 +6912,7 @@
         <v>866</v>
       </c>
       <c r="Q65" s="2" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
       <c r="R65" s="2" t="s">
         <v>23</v>
@@ -6965,7 +6968,7 @@
         <v>866</v>
       </c>
       <c r="Q66" s="1" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.2">
@@ -7018,7 +7021,7 @@
         <v>866</v>
       </c>
       <c r="Q67" s="2" t="s">
-        <v>946</v>
+        <v>942</v>
       </c>
     </row>
     <row r="68" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7068,7 +7071,7 @@
         <v>866</v>
       </c>
       <c r="Q68" s="1" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
     </row>
     <row r="69" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7118,7 +7121,7 @@
         <v>866</v>
       </c>
       <c r="Q69" s="1" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
     </row>
     <row r="70" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7168,7 +7171,7 @@
         <v>866</v>
       </c>
       <c r="Q70" s="1" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
     </row>
     <row r="71" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7265,7 +7268,7 @@
         <v>866</v>
       </c>
       <c r="Q72" s="1" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
     </row>
     <row r="73" spans="1:18" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
@@ -7315,7 +7318,7 @@
         <v>866</v>
       </c>
       <c r="Q73" s="1" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
     </row>
     <row r="74" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7362,10 +7365,10 @@
         <v>859</v>
       </c>
       <c r="P74" s="1" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="Q74" s="1" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="75" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -7617,10 +7620,10 @@
         <v>859</v>
       </c>
       <c r="P80" s="1" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="Q80" s="1" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
     </row>
     <row r="81" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8414,10 +8417,10 @@
         <v>859</v>
       </c>
       <c r="P99" s="1" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="Q99" s="1" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="100" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8514,7 +8517,7 @@
         <v>876</v>
       </c>
       <c r="Q101" s="1" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
     </row>
     <row r="102" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8561,10 +8564,10 @@
         <v>859</v>
       </c>
       <c r="P102" s="1" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="Q102" s="1" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
     </row>
     <row r="103" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8611,10 +8614,10 @@
         <v>859</v>
       </c>
       <c r="P103" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="Q103" s="1" t="s">
         <v>900</v>
-      </c>
-      <c r="Q103" s="1" t="s">
-        <v>902</v>
       </c>
     </row>
     <row r="104" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8661,10 +8664,10 @@
         <v>859</v>
       </c>
       <c r="P104" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="Q104" s="1" t="s">
         <v>900</v>
-      </c>
-      <c r="Q104" s="1" t="s">
-        <v>902</v>
       </c>
     </row>
     <row r="105" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8711,10 +8714,10 @@
         <v>859</v>
       </c>
       <c r="P105" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="Q105" s="1" t="s">
         <v>900</v>
-      </c>
-      <c r="Q105" s="1" t="s">
-        <v>902</v>
       </c>
     </row>
     <row r="106" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8761,10 +8764,10 @@
         <v>859</v>
       </c>
       <c r="P106" s="1" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="Q106" s="1" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
     </row>
     <row r="107" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8811,10 +8814,10 @@
         <v>859</v>
       </c>
       <c r="P107" s="1" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="Q107" s="1" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
     </row>
     <row r="108" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8861,10 +8864,10 @@
         <v>859</v>
       </c>
       <c r="P108" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="Q108" s="1" t="s">
         <v>900</v>
-      </c>
-      <c r="Q108" s="1" t="s">
-        <v>902</v>
       </c>
     </row>
     <row r="109" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8911,10 +8914,10 @@
         <v>859</v>
       </c>
       <c r="P109" s="1" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="Q109" s="1" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
     </row>
     <row r="110" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -8961,10 +8964,10 @@
         <v>859</v>
       </c>
       <c r="P110" s="1" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="Q110" s="1" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
     </row>
     <row r="111" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9014,7 +9017,7 @@
         <v>876</v>
       </c>
       <c r="Q111" s="1" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
     </row>
     <row r="112" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9111,10 +9114,10 @@
         <v>859</v>
       </c>
       <c r="P113" s="1" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="Q113" s="1" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
     </row>
     <row r="114" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9161,10 +9164,10 @@
         <v>859</v>
       </c>
       <c r="P114" s="1" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="Q114" s="1" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
     </row>
     <row r="115" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9211,10 +9214,10 @@
         <v>859</v>
       </c>
       <c r="P115" s="1" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="Q115" s="1" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
     </row>
     <row r="116" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9261,7 +9264,7 @@
         <v>859</v>
       </c>
       <c r="Q116" s="1" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
     </row>
     <row r="117" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9308,10 +9311,10 @@
         <v>859</v>
       </c>
       <c r="P117" s="1" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="Q117" s="1" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
     </row>
     <row r="118" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9358,10 +9361,10 @@
         <v>859</v>
       </c>
       <c r="P118" s="1" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="Q118" s="1" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.2">
@@ -9408,10 +9411,10 @@
         <v>856</v>
       </c>
       <c r="P119" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="Q119" s="2" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating wos176 big meta file
</commit_message>
<xml_diff>
--- a/data extraction /lit search metadata /wos176_final.xlsx
+++ b/data extraction /lit search metadata /wos176_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /lit search metadata /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012D9CFD-002C-D643-9CF1-74B98AB56E3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA4EA5A-0374-994E-9FA3-5645F45EF917}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="460" windowWidth="23980" windowHeight="11900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2400" yWindow="460" windowWidth="23980" windowHeight="11900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wos176_final" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1701" uniqueCount="948">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1702" uniqueCount="948">
   <si>
     <t>label</t>
   </si>
@@ -2795,9 +2795,6 @@
     <t>pulse press, acclimation experiment</t>
   </si>
   <si>
-    <t>heatshock, return for pulse press experiments work; missing sample size for current extraction</t>
-  </si>
-  <si>
     <t>might need to return to get actual irradiances for UV treatments (they manipulated both temperature and irradiance in these experiments)</t>
   </si>
   <si>
@@ -2843,9 +2840,6 @@
     <t>not sure about the f1 and f2 treatments features exposure to ambient temps? (eventhough they have the mean and range recorded)</t>
   </si>
   <si>
-    <t xml:space="preserve">unclear whther this should be considered multiple exposure or cold exposure--inclear whether there is a constant treatment to extract data frome </t>
-  </si>
-  <si>
     <t xml:space="preserve">return for cold exposure in figure 2 and figure 1; not sure how usable data for big met analysis is </t>
   </si>
   <si>
@@ -2865,6 +2859,12 @@
   </si>
   <si>
     <t xml:space="preserve">extracted figure 1 and 2, did not extract the offspring repsonse for figure 2 because did not appear normally distributed, calculated standard deviation from iqr and dividing by 1.35. not sure about sample sizes here </t>
+  </si>
+  <si>
+    <t xml:space="preserve">heatshock, return for pulse press experiments work; assumed sample size of 7 since methods said for each treatment n=7-9, assumed lower bound of sample size </t>
+  </si>
+  <si>
+    <t xml:space="preserve">extracted figure 2, excluded the temp directions of the same temp, not sure about sample size and not sure how to show the distinction between the the same ranges, one starting high and one starting low </t>
   </si>
 </sst>
 </file>
@@ -3719,8 +3719,8 @@
   <dimension ref="A1:R119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R67" sqref="R67"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5225,7 +5225,7 @@
         <v>866</v>
       </c>
       <c r="Q33" t="s">
-        <v>924</v>
+        <v>946</v>
       </c>
       <c r="R33" t="s">
         <v>23</v>
@@ -5281,7 +5281,7 @@
         <v>866</v>
       </c>
       <c r="Q34" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="R34" t="s">
         <v>23</v>
@@ -5387,7 +5387,7 @@
         <v>866</v>
       </c>
       <c r="Q36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="R36" t="s">
         <v>23</v>
@@ -5443,7 +5443,7 @@
         <v>876</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
@@ -5496,7 +5496,7 @@
         <v>866</v>
       </c>
       <c r="Q38" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="R38" t="s">
         <v>23</v>
@@ -5552,7 +5552,7 @@
         <v>866</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="R39" s="2" t="s">
         <v>23</v>
@@ -5658,7 +5658,7 @@
         <v>866</v>
       </c>
       <c r="Q41" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="R41" s="2" t="s">
         <v>23</v>
@@ -5820,7 +5820,7 @@
         <v>866</v>
       </c>
       <c r="Q44" s="2" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="R44" s="2" t="s">
         <v>23</v>
@@ -5876,7 +5876,7 @@
         <v>866</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="46" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5929,7 +5929,7 @@
         <v>876</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="47" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -5982,7 +5982,7 @@
         <v>866</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="48" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6138,7 +6138,7 @@
         <v>866</v>
       </c>
       <c r="Q50" s="2" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="R50" s="2" t="s">
         <v>23</v>
@@ -6194,7 +6194,7 @@
         <v>876</v>
       </c>
       <c r="Q51" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="R51" t="s">
         <v>23</v>
@@ -6297,7 +6297,7 @@
         <v>866</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
     </row>
     <row r="54" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6344,7 +6344,7 @@
         <v>859</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
     </row>
     <row r="55" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6444,7 +6444,7 @@
         <v>866</v>
       </c>
       <c r="Q56" s="2" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="R56" s="2" t="s">
         <v>23</v>
@@ -6547,7 +6547,10 @@
         <v>866</v>
       </c>
       <c r="Q58" s="2" t="s">
-        <v>940</v>
+        <v>947</v>
+      </c>
+      <c r="R58" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="59" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6600,7 +6603,7 @@
         <v>866</v>
       </c>
       <c r="Q59" s="1" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="60" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6700,7 +6703,7 @@
         <v>866</v>
       </c>
       <c r="Q61" s="1" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="62" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -6800,7 +6803,7 @@
         <v>866</v>
       </c>
       <c r="Q63" s="2" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="R63" s="2" t="s">
         <v>23</v>
@@ -6856,7 +6859,7 @@
         <v>866</v>
       </c>
       <c r="Q64" s="2" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="R64" s="2" t="s">
         <v>23</v>
@@ -6912,7 +6915,7 @@
         <v>866</v>
       </c>
       <c r="Q65" s="2" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="R65" s="2" t="s">
         <v>23</v>
@@ -6968,7 +6971,7 @@
         <v>866</v>
       </c>
       <c r="Q66" s="1" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.2">
@@ -7021,7 +7024,7 @@
         <v>866</v>
       </c>
       <c r="Q67" s="2" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="R67" s="2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
commiting to avoit merhe conflict
</commit_message>
<xml_diff>
--- a/data extraction /lit search metadata /wos176_final.xlsx
+++ b/data extraction /lit search metadata /wos176_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /lit search metadata /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA4EA5A-0374-994E-9FA3-5645F45EF917}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03ED1E3-5932-9241-931F-F760C2EEE979}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="460" windowWidth="23980" windowHeight="11900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2380" yWindow="460" windowWidth="23980" windowHeight="11900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wos176_final" sheetId="1" r:id="rId1"/>
@@ -3718,9 +3718,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R119"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H68" sqref="H68"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K101" sqref="K101:K119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7614,7 +7614,7 @@
         <v>21</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>188</v>
+        <v>409</v>
       </c>
       <c r="L80" s="1" t="s">
         <v>21</v>

</xml_diff>